<commit_message>
ebay add to cart
</commit_message>
<xml_diff>
--- a/com.ebay/src/test/resources/test_data_ebay.xlsx
+++ b/com.ebay/src/test/resources/test_data_ebay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdul\IdeaProjects\SeleniumBootcamp\com.ebay\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5E2651-175C-445F-8FC5-F43527B85509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2B7D8B-D6F6-4063-94BA-8B9C2C770861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{3A642AAC-DC96-4564-8337-F6684102E314}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>searchTerm</t>
   </si>
@@ -85,6 +85,18 @@
   </si>
   <si>
     <t>Auooz Akbar1996</t>
+  </si>
+  <si>
+    <t>anoor37290@gmail.com</t>
+  </si>
+  <si>
+    <t>Serpent9999+</t>
+  </si>
+  <si>
+    <t>justin.smith1@gmail.com</t>
+  </si>
+  <si>
+    <t>AydenLiam1213@</t>
   </si>
 </sst>
 </file>
@@ -560,7 +572,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4FA8403-6B38-412D-917A-897DCD2F9AEF}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -587,11 +599,28 @@
         <v>15</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{E702B3D3-C6EC-461E-9534-1D0C493C1CF1}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{BB286030-496F-4771-A8B5-BE717DB01453}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>